<commit_message>
open MySQL BVT test class
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1098" uniqueCount="564">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="578">
   <si>
     <t>Expected_result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2070,6 +2070,56 @@
   <si>
     <t>delete from $schema1 where id&gt;15</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_096</t>
+  </si>
+  <si>
+    <t>updel_097</t>
+  </si>
+  <si>
+    <t>两端范围删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键not between范围删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $schema1 where id&lt;5 or id&gt;15</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_096.csv</t>
+  </si>
+  <si>
+    <t>delete from $schema1 where id not between 10 and 11</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>19</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_098</t>
+  </si>
+  <si>
+    <t>delete from $schema1 where id not between 10 and 10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_097.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_098.csv</t>
   </si>
 </sst>
 </file>
@@ -2439,10 +2489,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L96"/>
+  <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="D64" workbookViewId="0">
-      <selection activeCell="K96" sqref="K96"/>
+      <selection activeCell="K99" sqref="K99"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -5961,6 +6011,111 @@
         <v>560</v>
       </c>
       <c r="L96" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="97" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A97" s="7" t="s">
+        <v>564</v>
+      </c>
+      <c r="B97" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C97" s="1" t="s">
+        <v>566</v>
+      </c>
+      <c r="D97" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F97" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="G97" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H97" s="1" t="s">
+        <v>568</v>
+      </c>
+      <c r="I97" s="1" t="s">
+        <v>569</v>
+      </c>
+      <c r="J97" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="K97" s="7" t="s">
+        <v>570</v>
+      </c>
+      <c r="L97" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="98" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A98" s="7" t="s">
+        <v>565</v>
+      </c>
+      <c r="B98" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C98" s="1" t="s">
+        <v>567</v>
+      </c>
+      <c r="D98" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F98" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="G98" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H98" s="1" t="s">
+        <v>571</v>
+      </c>
+      <c r="I98" s="1" t="s">
+        <v>572</v>
+      </c>
+      <c r="J98" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="K98" s="7" t="s">
+        <v>576</v>
+      </c>
+      <c r="L98" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A99" s="7" t="s">
+        <v>573</v>
+      </c>
+      <c r="B99" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C99" s="7" t="s">
+        <v>567</v>
+      </c>
+      <c r="D99" s="7" t="s">
+        <v>153</v>
+      </c>
+      <c r="F99" s="7" t="s">
+        <v>545</v>
+      </c>
+      <c r="G99" s="7" t="s">
+        <v>345</v>
+      </c>
+      <c r="H99" s="7" t="s">
+        <v>574</v>
+      </c>
+      <c r="I99" s="7" t="s">
+        <v>575</v>
+      </c>
+      <c r="J99" s="7" t="s">
+        <v>554</v>
+      </c>
+      <c r="K99" s="7" t="s">
+        <v>577</v>
+      </c>
+      <c r="L99" s="7" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
open data provider run in parallel
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -2155,12 +2155,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -2175,7 +2181,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -2184,6 +2190,7 @@
     <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="常规" xfId="0" builtinId="0"/>
@@ -2488,7 +2495,7 @@
   <dimension ref="A1:L99"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K2" sqref="K2"/>
+      <selection activeCell="C82" sqref="C82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -4851,7 +4858,7 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A66" s="7" t="s">
+      <c r="A66" s="8" t="s">
         <v>303</v>
       </c>
       <c r="B66" s="7" t="s">
@@ -4889,7 +4896,7 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A67" s="7" t="s">
+      <c r="A67" s="8" t="s">
         <v>304</v>
       </c>
       <c r="B67" s="7" t="s">
@@ -4927,7 +4934,7 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A68" s="7" t="s">
+      <c r="A68" s="8" t="s">
         <v>315</v>
       </c>
       <c r="B68" s="7" t="s">
@@ -4965,7 +4972,7 @@
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A69" s="7" t="s">
+      <c r="A69" s="8" t="s">
         <v>316</v>
       </c>
       <c r="B69" s="7" t="s">
@@ -5003,7 +5010,7 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A70" s="7" t="s">
+      <c r="A70" s="8" t="s">
         <v>324</v>
       </c>
       <c r="B70" s="7" t="s">
@@ -5041,7 +5048,7 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A71" s="7" t="s">
+      <c r="A71" s="8" t="s">
         <v>325</v>
       </c>
       <c r="B71" s="7" t="s">
@@ -5079,7 +5086,7 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A72" s="7" t="s">
+      <c r="A72" s="8" t="s">
         <v>326</v>
       </c>
       <c r="B72" s="7" t="s">
@@ -5117,7 +5124,7 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A73" s="7" t="s">
+      <c r="A73" s="8" t="s">
         <v>327</v>
       </c>
       <c r="B73" s="7" t="s">
@@ -5155,7 +5162,7 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A74" s="7" t="s">
+      <c r="A74" s="8" t="s">
         <v>328</v>
       </c>
       <c r="B74" s="7" t="s">
@@ -5193,7 +5200,7 @@
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A75" s="7" t="s">
+      <c r="A75" s="8" t="s">
         <v>329</v>
       </c>
       <c r="B75" s="7" t="s">
@@ -5231,7 +5238,7 @@
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A76" s="7" t="s">
+      <c r="A76" s="8" t="s">
         <v>330</v>
       </c>
       <c r="B76" s="7" t="s">
@@ -5269,7 +5276,7 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A77" s="7" t="s">
+      <c r="A77" s="8" t="s">
         <v>331</v>
       </c>
       <c r="B77" s="7" t="s">
@@ -5307,7 +5314,7 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A78" s="7" t="s">
+      <c r="A78" s="8" t="s">
         <v>332</v>
       </c>
       <c r="B78" s="7" t="s">
@@ -5345,7 +5352,7 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A79" s="7" t="s">
+      <c r="A79" s="8" t="s">
         <v>333</v>
       </c>
       <c r="B79" s="7" t="s">
@@ -5383,7 +5390,7 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A80" s="7" t="s">
+      <c r="A80" s="8" t="s">
         <v>334</v>
       </c>
       <c r="B80" s="7" t="s">
@@ -5421,7 +5428,7 @@
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A81" s="7" t="s">
+      <c r="A81" s="8" t="s">
         <v>335</v>
       </c>
       <c r="B81" s="7" t="s">
@@ -5459,7 +5466,7 @@
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A82" s="7" t="s">
+      <c r="A82" s="8" t="s">
         <v>336</v>
       </c>
       <c r="B82" s="7" t="s">
@@ -5649,7 +5656,7 @@
       </c>
     </row>
     <row r="87" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A87" s="7" t="s">
+      <c r="A87" s="8" t="s">
         <v>424</v>
       </c>
       <c r="B87" s="7" t="s">
@@ -5687,7 +5694,7 @@
       </c>
     </row>
     <row r="88" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A88" s="7" t="s">
+      <c r="A88" s="8" t="s">
         <v>425</v>
       </c>
       <c r="B88" s="7" t="s">
@@ -5725,7 +5732,7 @@
       </c>
     </row>
     <row r="89" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A89" s="7" t="s">
+      <c r="A89" s="8" t="s">
         <v>436</v>
       </c>
       <c r="B89" s="7" t="s">
@@ -5763,7 +5770,7 @@
       </c>
     </row>
     <row r="90" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A90" s="7" t="s">
+      <c r="A90" s="8" t="s">
         <v>437</v>
       </c>
       <c r="B90" s="7" t="s">

</xml_diff>

<commit_message>
add delete/update in multi-partition table and release negative cases about array
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1131" uniqueCount="578">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1175" uniqueCount="601">
   <si>
     <t>Expected_result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2116,6 +2116,90 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_098.csv</t>
+  </si>
+  <si>
+    <t>updel_099</t>
+  </si>
+  <si>
+    <t>updel_100</t>
+  </si>
+  <si>
+    <t>多分区条件删除，小于条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区条件删除，大于条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>schema9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_value04</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $schema9 where id&lt;100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $schema9 where id&gt;0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $schema9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_099.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_100.csv</t>
+  </si>
+  <si>
+    <t>10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_101</t>
+  </si>
+  <si>
+    <t>updel_102</t>
+  </si>
+  <si>
+    <t>多分区条件更新，小于条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>多分区条件更新，大于条件</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $schema9 set name='Java' where id&lt;20</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>6</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_101.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_102.csv</t>
+  </si>
+  <si>
+    <t>8</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $schema9 set amount=99.99 where id&gt;=10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2492,10 +2576,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L99"/>
+  <dimension ref="A1:L103"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A58" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66:B82"/>
+    <sheetView tabSelected="1" topLeftCell="A76" workbookViewId="0">
+      <selection activeCell="I106" sqref="I106"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6119,6 +6203,148 @@
         <v>577</v>
       </c>
       <c r="L99" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="100" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A100" s="7" t="s">
+        <v>578</v>
+      </c>
+      <c r="B100" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C100" s="1" t="s">
+        <v>580</v>
+      </c>
+      <c r="D100" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F100" s="1" t="s">
+        <v>582</v>
+      </c>
+      <c r="G100" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="H100" s="1" t="s">
+        <v>584</v>
+      </c>
+      <c r="I100" s="1" t="s">
+        <v>586</v>
+      </c>
+      <c r="J100" s="1" t="s">
+        <v>587</v>
+      </c>
+      <c r="K100" s="7" t="s">
+        <v>588</v>
+      </c>
+      <c r="L100" s="1" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="101" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A101" s="7" t="s">
+        <v>579</v>
+      </c>
+      <c r="B101" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C101" s="7" t="s">
+        <v>581</v>
+      </c>
+      <c r="D101" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F101" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="G101" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="H101" s="1" t="s">
+        <v>585</v>
+      </c>
+      <c r="I101" s="1" t="s">
+        <v>590</v>
+      </c>
+      <c r="J101" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="K101" s="7" t="s">
+        <v>589</v>
+      </c>
+      <c r="L101" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A102" s="7" t="s">
+        <v>591</v>
+      </c>
+      <c r="B102" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C102" s="7" t="s">
+        <v>593</v>
+      </c>
+      <c r="D102" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E102" s="7"/>
+      <c r="F102" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="G102" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="H102" s="1" t="s">
+        <v>595</v>
+      </c>
+      <c r="I102" s="1" t="s">
+        <v>596</v>
+      </c>
+      <c r="J102" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="K102" s="7" t="s">
+        <v>597</v>
+      </c>
+      <c r="L102" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="103" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A103" s="7" t="s">
+        <v>592</v>
+      </c>
+      <c r="B103" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C103" s="7" t="s">
+        <v>594</v>
+      </c>
+      <c r="D103" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E103" s="7"/>
+      <c r="F103" s="7" t="s">
+        <v>582</v>
+      </c>
+      <c r="G103" s="7" t="s">
+        <v>583</v>
+      </c>
+      <c r="H103" s="7" t="s">
+        <v>600</v>
+      </c>
+      <c r="I103" s="1" t="s">
+        <v>599</v>
+      </c>
+      <c r="J103" s="7" t="s">
+        <v>587</v>
+      </c>
+      <c r="K103" s="7" t="s">
+        <v>598</v>
+      </c>
+      <c r="L103" s="7" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add mix index test method
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1223" uniqueCount="633">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="651">
   <si>
     <t>Expected_result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2229,10 +2229,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>400</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_103.csv</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -2320,6 +2316,76 @@
   </si>
   <si>
     <t>update $scalar047 set gmt=1234</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_107</t>
+  </si>
+  <si>
+    <t>9</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_108</t>
+  </si>
+  <si>
+    <t>带有向量索引的表更新数值标量字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>带有向量索引的表更新字符标量字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_109</t>
+  </si>
+  <si>
+    <t>带有向量索引的表更新日期标量字段</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $vector062 set address='beijing' where id in (10,20,30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>3</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $vector062 set birthday='2023-09-20' where id=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,address from $vector062 where id in (10,20,30)</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,birthday from $vector062 where id=100</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_107.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_108.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_109.csv</t>
+  </si>
+  <si>
+    <t>update $vector062 set amount=1234.1234 where id&lt;10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,amount from $vector062 where id&lt;10</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>490</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2697,10 +2763,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L107"/>
+  <dimension ref="A1:L110"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D82" workbookViewId="0">
-      <selection activeCell="J107" sqref="J107"/>
+    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6495,13 +6561,13 @@
         <v>607</v>
       </c>
       <c r="I104" s="1" t="s">
+        <v>650</v>
+      </c>
+      <c r="J104" s="1" t="s">
+        <v>609</v>
+      </c>
+      <c r="K104" s="7" t="s">
         <v>608</v>
-      </c>
-      <c r="J104" s="1" t="s">
-        <v>610</v>
-      </c>
-      <c r="K104" s="7" t="s">
-        <v>609</v>
       </c>
       <c r="L104" s="1" t="s">
         <v>19</v>
@@ -6509,37 +6575,37 @@
     </row>
     <row r="105" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A105" s="7" t="s">
-        <v>611</v>
+        <v>610</v>
       </c>
       <c r="B105" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C105" s="1" t="s">
+        <v>612</v>
+      </c>
+      <c r="D105" s="1" t="s">
         <v>613</v>
       </c>
-      <c r="D105" s="1" t="s">
+      <c r="E105" s="1" t="s">
         <v>614</v>
       </c>
-      <c r="E105" s="1" t="s">
+      <c r="F105" s="1" t="s">
         <v>615</v>
       </c>
-      <c r="F105" s="1" t="s">
+      <c r="G105" s="1" t="s">
         <v>616</v>
       </c>
-      <c r="G105" s="1" t="s">
+      <c r="H105" s="1" t="s">
+        <v>619</v>
+      </c>
+      <c r="I105" s="1" t="s">
         <v>617</v>
       </c>
-      <c r="H105" s="1" t="s">
+      <c r="J105" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="K105" s="7" t="s">
         <v>620</v>
-      </c>
-      <c r="I105" s="1" t="s">
-        <v>618</v>
-      </c>
-      <c r="J105" s="1" t="s">
-        <v>619</v>
-      </c>
-      <c r="K105" s="7" t="s">
-        <v>621</v>
       </c>
       <c r="L105" s="7" t="s">
         <v>19</v>
@@ -6547,37 +6613,37 @@
     </row>
     <row r="106" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A106" s="7" t="s">
-        <v>612</v>
+        <v>611</v>
       </c>
       <c r="B106" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C106" s="1" t="s">
-        <v>623</v>
+        <v>622</v>
       </c>
       <c r="D106" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="E106" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="E106" s="7" t="s">
+      <c r="F106" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="F106" s="7" t="s">
+      <c r="G106" s="7" t="s">
         <v>616</v>
       </c>
-      <c r="G106" s="7" t="s">
-        <v>617</v>
-      </c>
       <c r="H106" s="1" t="s">
+        <v>625</v>
+      </c>
+      <c r="I106" s="1" t="s">
+        <v>624</v>
+      </c>
+      <c r="J106" s="1" t="s">
         <v>626</v>
       </c>
-      <c r="I106" s="1" t="s">
-        <v>625</v>
-      </c>
-      <c r="J106" s="1" t="s">
+      <c r="K106" s="7" t="s">
         <v>627</v>
-      </c>
-      <c r="K106" s="7" t="s">
-        <v>628</v>
       </c>
       <c r="L106" s="7" t="s">
         <v>19</v>
@@ -6585,39 +6651,153 @@
     </row>
     <row r="107" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A107" s="7" t="s">
-        <v>622</v>
+        <v>621</v>
       </c>
       <c r="B107" s="7" t="s">
         <v>11</v>
       </c>
       <c r="C107" s="7" t="s">
-        <v>624</v>
+        <v>623</v>
       </c>
       <c r="D107" s="7" t="s">
+        <v>613</v>
+      </c>
+      <c r="E107" s="7" t="s">
         <v>614</v>
       </c>
-      <c r="E107" s="7" t="s">
+      <c r="F107" s="7" t="s">
         <v>615</v>
       </c>
-      <c r="F107" s="7" t="s">
+      <c r="G107" s="7" t="s">
         <v>616</v>
       </c>
-      <c r="G107" s="7" t="s">
-        <v>617</v>
-      </c>
       <c r="H107" s="7" t="s">
+        <v>631</v>
+      </c>
+      <c r="I107" s="1" t="s">
+        <v>629</v>
+      </c>
+      <c r="J107" s="1" t="s">
+        <v>630</v>
+      </c>
+      <c r="K107" s="7" t="s">
+        <v>628</v>
+      </c>
+      <c r="L107" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="108" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A108" s="7" t="s">
         <v>632</v>
       </c>
-      <c r="I107" s="1" t="s">
-        <v>630</v>
-      </c>
-      <c r="J107" s="1" t="s">
-        <v>631</v>
-      </c>
-      <c r="K107" s="7" t="s">
-        <v>629</v>
-      </c>
-      <c r="L107" s="7" t="s">
+      <c r="B108" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C108" s="1" t="s">
+        <v>635</v>
+      </c>
+      <c r="D108" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E108" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="F108" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="G108" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="H108" s="1" t="s">
+        <v>648</v>
+      </c>
+      <c r="I108" s="1" t="s">
+        <v>633</v>
+      </c>
+      <c r="J108" s="1" t="s">
+        <v>649</v>
+      </c>
+      <c r="K108" s="7" t="s">
+        <v>645</v>
+      </c>
+      <c r="L108" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="109" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A109" s="7" t="s">
+        <v>634</v>
+      </c>
+      <c r="B109" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C109" s="7" t="s">
+        <v>636</v>
+      </c>
+      <c r="D109" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E109" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="F109" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="G109" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="H109" s="7" t="s">
+        <v>639</v>
+      </c>
+      <c r="I109" s="1" t="s">
+        <v>640</v>
+      </c>
+      <c r="J109" s="1" t="s">
+        <v>643</v>
+      </c>
+      <c r="K109" s="7" t="s">
+        <v>646</v>
+      </c>
+      <c r="L109" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="110" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A110" s="7" t="s">
+        <v>637</v>
+      </c>
+      <c r="B110" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C110" s="7" t="s">
+        <v>638</v>
+      </c>
+      <c r="D110" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E110" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="F110" s="7" t="s">
+        <v>605</v>
+      </c>
+      <c r="G110" s="7" t="s">
+        <v>606</v>
+      </c>
+      <c r="H110" s="7" t="s">
+        <v>642</v>
+      </c>
+      <c r="I110" s="1" t="s">
+        <v>641</v>
+      </c>
+      <c r="J110" s="1" t="s">
+        <v>644</v>
+      </c>
+      <c r="K110" s="7" t="s">
+        <v>647</v>
+      </c>
+      <c r="L110" s="7" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add case about update scalar index filtered by its own value
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1259" uniqueCount="651">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="664">
   <si>
     <t>Expected_result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2387,6 +2387,54 @@
   <si>
     <t>490</t>
     <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_110</t>
+  </si>
+  <si>
+    <t>updel_111</t>
+  </si>
+  <si>
+    <t>scalar055</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>scalar055_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $scalar055 set amount=888.88 where amount=279540.148</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar055 where amount=888.88</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_110.csv</t>
+  </si>
+  <si>
+    <t>更新标量索引字段值通过标量索引字段过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>更新标量索引字段值通过主键字段过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $scalar055 set amount=-999.999 where id=4695</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar055 where amount=-999.999</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_111.csv</t>
   </si>
 </sst>
 </file>
@@ -2763,10 +2811,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L110"/>
+  <dimension ref="A1:L112"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A82" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
+      <selection activeCell="G123" sqref="G123"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2778,7 +2826,7 @@
     <col min="5" max="5" width="11.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="47.75" style="1" customWidth="1"/>
+    <col min="8" max="8" width="60.625" style="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38" style="1" customWidth="1"/>
     <col min="11" max="12" width="19.5" style="1" bestFit="1" customWidth="1"/>
@@ -6798,6 +6846,82 @@
         <v>647</v>
       </c>
       <c r="L110" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="111" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A111" s="7" t="s">
+        <v>651</v>
+      </c>
+      <c r="B111" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C111" s="1" t="s">
+        <v>659</v>
+      </c>
+      <c r="D111" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E111" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="F111" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="G111" s="1" t="s">
+        <v>654</v>
+      </c>
+      <c r="H111" s="1" t="s">
+        <v>655</v>
+      </c>
+      <c r="I111" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="J111" s="1" t="s">
+        <v>657</v>
+      </c>
+      <c r="K111" s="7" t="s">
+        <v>658</v>
+      </c>
+      <c r="L111" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A112" s="7" t="s">
+        <v>652</v>
+      </c>
+      <c r="B112" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C112" s="7" t="s">
+        <v>660</v>
+      </c>
+      <c r="D112" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E112" s="7" t="s">
+        <v>614</v>
+      </c>
+      <c r="F112" s="7" t="s">
+        <v>653</v>
+      </c>
+      <c r="G112" s="7" t="s">
+        <v>654</v>
+      </c>
+      <c r="H112" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="I112" s="1" t="s">
+        <v>656</v>
+      </c>
+      <c r="J112" s="7" t="s">
+        <v>662</v>
+      </c>
+      <c r="K112" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="L112" s="7" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>

<commit_message>
add case about query vector after data delete
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1283" uniqueCount="664">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1295" uniqueCount="672">
   <si>
     <t>Expected_result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2435,6 +2435,36 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_111.csv</t>
+  </si>
+  <si>
+    <t>updel_112</t>
+  </si>
+  <si>
+    <t>向量表删除后后置过滤</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mix018_value1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>mixindex018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $mixindex018</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_112.csv</t>
+  </si>
+  <si>
+    <t>select id,age,gender,hobby,color_index$distance from vector($mixindex018, color, array[0.009107396006584167,-0.4928479492664337,-0.06084398180246353,0.11279209703207016,0.42720580101013184,-0.5535244345664978,-0.051339954137802124,0.3442928194999695,0.397807240486145,0.14437393844127655,-0.27258825302124023,0.11299128085374832,0.26662662625312805,-0.3028406798839569,-0.06034494936466217,-0.20874223113059998,0.710351824760437,0.03114473819732666,-0.10010837763547897,-0.499957799911499,-0.3172328472137451,0.18967600166797638,0.16708506643772125,-0.31831443309783936,-0.3038794696331024,0.517365038394928,-0.1310274302959442,0.6051051020622253,-0.29701799154281616,-0.11700791120529175,-0.49527180194854736,0.3499431014060974,-0.05310584604740143,0.11840163171291351,-0.6476613283157349,-0.40672868490219116,0.15504536032676697,-0.04425550997257233,-0.017758861184120178,-0.4650961756706238,-0.367722749710083,0.4912892282009125,0.15679343044757843,-1.2024909257888794,-0.6475555896759033,0.8445031642913818,-0.3021777868270874,0.0012783706188201904,-0.1028386726975441,-0.028430849313735962,0.4390820562839508,0.17291557788848877,0.02308507263660431,-0.2666246294975281,0.030758768320083618,0.3070322275161743,0.7922346591949463,0.15251073241233826,0.3876311779022217,-0.12918725609779358,0.5775445699691772,0.13809040188789368,0.3011755347251892,-0.08841019868850708,-0.2804226875305176,0.08000586181879044,0.23992058634757996,0.30137330293655396,-0.573534369468689,-0.08557131141424179,-0.009991265833377838,0.22057701647281647,-0.07465316355228424,-0.1380939483642578,0.12757709622383118,-0.1524963080883026,-0.21346122026443481,-0.21207493543624878,-0.299119770526886,-0.105656199157238,0.2978556156158447,0.27103662490844727,-0.04677818715572357,-0.25942736864089966,0.23926180601119995,0.06485702842473984,-0.2326173037290573,-0.7795956134796143,0.5515224933624268,-0.13598020374774933,-0.3016166687011719,-0.23002196848392487,-5.020496845245361,1.1768553256988525,0.04210896044969559,0.05429087206721306,-0.12462489306926727,-0.2512921392917633,0.025492563843727112,-0.014712274074554443,0.3395729660987854,0.36077940464019775,0.710265040397644,0.5866747498512268,0.3867844343185425,0.16563571989536285,-2.2621219158172607,-0.31919386982917786,-0.29929596185684204,-0.1239459365606308,-0.019464053213596344,-0.18152916431427002,0.015370100736618042,-0.39437994360923767,-0.3952904939651489,-0.17863686382770538,0.3756665587425232,0.01915770024061203,-0.0487205907702446,0.5403110980987549,0.13948170840740204,0.7490887641906738,0.218780517578125,0.21333663165569305,0.6106190085411072,-0.5787690877914429,0.005233213305473328,-0.02014821767807007,-0.37207454442977905,0.04737117886543274,0.3805462121963501,0.022129982709884644,-0.08685516566038132,0.8918148279190063,0.332944393157959,-0.17890742421150208,-0.01971307396888733,-0.49113523960113525,-0.16974413394927979,0.29028767347335815,-0.0854928120970726,-0.28040117025375366,0.27752572298049927,0.19523702561855316,-0.010701179504394531,0.41232433915138245,-0.2981152832508087,0.17831067740917206,0.23491880297660828,0.5166872143745422,0.03726338595151901,-0.09167103469371796,-0.14614176750183105,0.0835254117846489,-0.526052713394165,0.5634927749633789,0.4244139492511749,0.08627873659133911,0.11286911368370056,-0.09144455194473267,0.19640317559242249,-0.28446879982948303,-0.14722681045532227,-0.15440787374973297,0.38722527027130127,0.2799495756626129,0.2579476833343506,0.07801324129104614,-0.03614184260368347,0.2691837549209595,-0.22063779830932617,0.20414650440216064,0.290392130613327,-0.23576216399669647,0.6217473745346069,-0.36090806126594543,-0.5171005129814148,-0.0978025570511818,-0.22199128568172455,0.11597487330436707,-0.10627104341983795,0.0140666663646698,-0.3552021086215973,0.04552648216485977,0.028643697500228882,-0.2697099447250366,-0.08528557419776917,-0.3565848469734192,-0.6836068034172058,0.4241693317890167,0.3769601583480835,-0.3473547399044037,-0.28350770473480225,0.4194734990596771,0.16857166588306427,0.24369701743125916,0.7187827229499817,-0.24069659411907196,-0.612932026386261,-0.02567557990550995,0.025800958275794983,-0.2763204872608185,0.06153678894042969,0.42983344197273254,-0.27653318643569946,0.07124429941177368,-0.21047277748584747,-0.19868281483650208,-0.40652528405189514,-0.2593531012535095,0.35989561676979065,0.7571883797645569,0.6407842636108398,0.29625385999679565,0.4905804395675659,-0.11757611483335495,-0.15926161408424377,0.05945210158824921,0.9470091462135315,-0.2651394009590149,0.24507103860378265,0.012639820575714111,-0.16477082669734955,0.023227810859680176,0.3517795503139496,0.061285004019737244,0.23400992155075073,-0.004913773387670517,0.10474497079849243,0.28454095125198364,0.2646726965904236,0.056223608553409576,0.14024418592453003,0.09913889318704605,0.37895309925079346,0.4080517888069153,0.23690679669380188,-0.9799992442131042,0.6079041361808777,-0.8063328862190247,-0.18007591366767883,0.4238743185997009,0.5677311420440674,0.07879464328289032,-0.6451236009597778,0.3615572452545166,-0.6502392292022705,-0.13250525295734406,0.022514693439006805,0.23416417837142944,-0.31921306252479553,0.015400782227516174,0.3049747347831726,-0.49025920033454895,0.6232213377952576,-0.17872992157936096,0.22888170182704926,0.06563788652420044,-0.09811440110206604,0.5739450454711914,0.19145318865776062,0.19296371936798096,0.1447419375181198,0.6271354556083679,-0.40667158365249634,0.14535176753997803,0.08282049000263214,-0.2226463258266449,0.19218046963214874,0.18990464508533478,0.366453617811203,0.1181904524564743,0.31326085329055786,0.2777858078479767,0.18976512551307678,0.12058664858341217,0.3834364712238312,-0.25943732261657715,0.15866270661354065,-0.14582546055316925,0.2993849217891693,0.3625524640083313,-0.5657874345779419,0.3584221601486206,0.6659886837005615,0.5365152359008789,0.15160009264945984,-0.0038372427225112915,-0.03198322653770447,-0.41171130537986755,0.35392409563064575,0.4899391531944275,-0.44131115078926086,-0.03127241134643555,-0.08564724773168564,-0.2810729742050171,-0.1650094985961914,0.41276872158050537,-0.20266728103160858,-0.21721073985099792,0.06289903819561005,-0.1000848263502121,0.3060847520828247,-0.1798524409532547,-0.053416907787323,-0.17533081769943237,0.4803808927536011,0.6472082734107971,-0.20990946888923645,-0.08272083848714828,0.2603752315044403,0.2435430884361267,0.8928165435791016,0.04669277369976044,0.06500576436519623,0.0932016521692276,0.4320862591266632,-0.19006873667240143,-0.4583078622817993,-0.06959453225135803,0.41687387228012085,1.279518961906433,-0.09231052547693253,0.39603978395462036,0.4426204264163971,0.1414766013622284,0.14081603288650513,0.029098331928253174,-0.0008250568062067032,-0.04960125684738159,0.10457373410463333,0.5750452876091003,-0.23702768981456757,0.07400791347026825,-0.39593395590782166,0.2875250577926636,0.40632858872413635,0.4273437261581421,-0.15563148260116577,-0.1943039447069168,0.09682011604309082,0.2771073579788208,-0.17696169018745422,-0.15394936501979828,-0.028617314994335175,-0.6125500202178955,0.055850833654403687,-0.33313047885894775,-0.18644365668296814,0.05475170910358429,0.08947843313217163,-0.07653182744979858,0.09828981757164001,-0.03744521737098694,-0.09890225529670715,0.3104325830936432,0.3743216395378113,0.7847214937210083,0.22328320145606995,-0.007173389196395874,0.2743714451789856,0.3419463038444519,-0.4041624963283539,0.8219678401947021,-0.937566339969635,-0.0877365693449974,0.08319441229104996,0.519494891166687,0.14611385762691498,0.6832436919212341,0.08052428811788559,0.4532940685749054,-0.11158505082130432,0.05747853219509125,-0.03627094626426697,0.29975807666778564,0.3184080719947815,-0.15185518562793732,-0.17107611894607544,-0.26622259616851807,-0.041283462196588516,0.2775959074497223,0.5768389701843262,-0.19857929646968842,-0.383053183555603,-0.4868699014186859,0.3679580092430115,0.31410154700279236,0.45399945974349976,0.565982460975647,-0.9887039661407471,-0.5410878658294678,-0.25793322920799255,-0.4151421785354614,0.9581260085105896,0.08737964928150177,0.12770259380340576,0.17853334546089172,-0.47929897904396057,-0.18773919343948364,-0.06778784096240997,0.2790369987487793,0.3038453459739685,-0.00035012513399124146,0.21557708084583282,-0.2987268567085266,-0.37862226366996765,0.11563920229673386,0.37216106057167053,0.07540548592805862,-0.14644283056259155,0.36704716086387634,0.27644112706184387,0.23733626306056976,-0.15499460697174072,0.18270283937454224,0.286896288394928,0.0611887089908123,-0.003465220332145691,-0.44345101714134216,-0.48094767332077026,-0.05870349705219269,0.2203047126531601,0.23658716678619385,0.14524224400520325,-0.3096632957458496,-0.42239847779273987,0.14180953800678253,-1.9080333709716797,0.7268998026847839,0.21734172105789185,0.3595874309539795,-0.24850676953792572,-0.0687989890575409,-0.2876971960067749,-0.008909806609153748,0.06251184642314911,0.17282895743846893,-0.24134333431720734,-0.34526604413986206,-0.6466650366783142,0.42585867643356323,0.5730605125427246,0.02659779042005539,0.3097115755081177,0.29858189821243286,-0.07963889837265015,-0.2749827802181244,-0.03155626356601715,-0.037864506244659424,0.11886607110500336,0.0742151141166687,0.454728901386261,0.11392711102962494,-0.0018827617168426514,-0.6696452498435974,0.3057352304458618,0.18775613605976105,0.07171911001205444,0.1750405877828598,-0.2657383978366852,0.24411165714263916,0.2512362003326416,-0.10027620196342468,0.3601529002189636,0.37912803888320923,-0.06990914046764374,-0.3299768567085266,-0.125762477517128,-0.2828892767429352,0.15549014508724213,0.13161194324493408,0.39875492453575134,-0.4680383801460266,-0.13426533341407776,0.2584708333015442,0.01619536429643631,0.26572245359420776,-0.3058027923107147,0.0349903404712677,-0.5298135280609131,-0.5118231177330017,0.35788029432296753,0.25099503993988037,-0.3409276306629181,0.0350998193025589,0.12917760014533997,0.04360932856798172,0.03863629698753357,-0.12423983961343765,-0.44539687037467957,0.06586220115423203,0.29936468601226807,-0.7707462310791016,-0.130367249250412,0.18743553757667542,-0.2837158441543579,0.07794137299060822,-0.24770815670490265,0.4286563992500305,-0.13582590222358704,0.13121500611305237,-0.001750364899635315,0.3049774765968323,-0.39047953486442566,0.24318626523017883,-0.4263252913951874,0.2714003324508667,0.17210617661476135,0.6087738871574402,-0.18345880508422852,0.11825743317604065], 10) where age&gt;1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2811,10 +2841,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L112"/>
+  <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A88" workbookViewId="0">
-      <selection activeCell="B115" sqref="B115"/>
+    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
+      <selection activeCell="B105" sqref="B105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2876,7 +2906,7 @@
         <v>227</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -2914,7 +2944,7 @@
         <v>228</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -2952,7 +2982,7 @@
         <v>229</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
@@ -2990,7 +3020,7 @@
         <v>230</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>27</v>
@@ -3028,7 +3058,7 @@
         <v>231</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3063,7 +3093,7 @@
         <v>232</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -3098,7 +3128,7 @@
         <v>233</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>56</v>
@@ -3133,7 +3163,7 @@
         <v>234</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>57</v>
@@ -3168,7 +3198,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>58</v>
@@ -3204,7 +3234,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>59</v>
@@ -3240,7 +3270,7 @@
         <v>237</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>55</v>
@@ -3276,7 +3306,7 @@
         <v>238</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>60</v>
@@ -3312,7 +3342,7 @@
         <v>239</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>61</v>
@@ -3348,7 +3378,7 @@
         <v>240</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>62</v>
@@ -3384,7 +3414,7 @@
         <v>241</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>74</v>
@@ -3420,7 +3450,7 @@
         <v>242</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>77</v>
@@ -3456,7 +3486,7 @@
         <v>243</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>81</v>
@@ -3492,7 +3522,7 @@
         <v>244</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>82</v>
@@ -3528,7 +3558,7 @@
         <v>245</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>83</v>
@@ -3564,7 +3594,7 @@
         <v>246</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>84</v>
@@ -3600,7 +3630,7 @@
         <v>247</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>92</v>
@@ -3635,7 +3665,7 @@
         <v>248</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>92</v>
@@ -3670,7 +3700,7 @@
         <v>249</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>92</v>
@@ -3705,7 +3735,7 @@
         <v>250</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>92</v>
@@ -3740,7 +3770,7 @@
         <v>251</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>92</v>
@@ -3775,7 +3805,7 @@
         <v>252</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>92</v>
@@ -3810,7 +3840,7 @@
         <v>253</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>110</v>
@@ -3845,7 +3875,7 @@
         <v>254</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>110</v>
@@ -3881,7 +3911,7 @@
         <v>255</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>110</v>
@@ -3917,7 +3947,7 @@
         <v>256</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>110</v>
@@ -3953,7 +3983,7 @@
         <v>257</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>127</v>
@@ -3991,7 +4021,7 @@
         <v>258</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>128</v>
@@ -4029,7 +4059,7 @@
         <v>259</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>129</v>
@@ -4067,7 +4097,7 @@
         <v>260</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>153</v>
@@ -4105,7 +4135,7 @@
         <v>261</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>154</v>
@@ -4143,7 +4173,7 @@
         <v>262</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>130</v>
@@ -4181,7 +4211,7 @@
         <v>263</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>131</v>
@@ -4219,7 +4249,7 @@
         <v>264</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>132</v>
@@ -4257,7 +4287,7 @@
         <v>265</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>133</v>
@@ -4295,7 +4325,7 @@
         <v>266</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>134</v>
@@ -4333,7 +4363,7 @@
         <v>267</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>135</v>
@@ -4371,7 +4401,7 @@
         <v>268</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>160</v>
@@ -4409,7 +4439,7 @@
         <v>269</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>162</v>
@@ -4447,7 +4477,7 @@
         <v>270</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>125</v>
@@ -4485,7 +4515,7 @@
         <v>271</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>168</v>
@@ -4523,7 +4553,7 @@
         <v>272</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>177</v>
@@ -4561,7 +4591,7 @@
         <v>273</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>206</v>
@@ -4599,7 +4629,7 @@
         <v>274</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>205</v>
@@ -4637,7 +4667,7 @@
         <v>275</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>209</v>
@@ -4675,7 +4705,7 @@
         <v>276</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>208</v>
@@ -4713,7 +4743,7 @@
         <v>277</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>211</v>
@@ -4751,7 +4781,7 @@
         <v>278</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>210</v>
@@ -4789,7 +4819,7 @@
         <v>279</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>213</v>
@@ -4827,7 +4857,7 @@
         <v>280</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>212</v>
@@ -4865,7 +4895,7 @@
         <v>281</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>181</v>
@@ -4903,7 +4933,7 @@
         <v>282</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>182</v>
@@ -4941,7 +4971,7 @@
         <v>283</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>190</v>
@@ -4970,7 +5000,7 @@
         <v>284</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>190</v>
@@ -4999,7 +5029,7 @@
         <v>285</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>192</v>
@@ -5026,7 +5056,7 @@
         <v>286</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>191</v>
@@ -5055,7 +5085,7 @@
         <v>287</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>191</v>
@@ -5084,7 +5114,7 @@
         <v>288</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>193</v>
@@ -5111,7 +5141,7 @@
         <v>291</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>292</v>
@@ -5146,7 +5176,7 @@
         <v>298</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>299</v>
@@ -5177,11 +5207,11 @@
       </c>
     </row>
     <row r="66" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A66" s="8" t="s">
+      <c r="A66" s="7" t="s">
         <v>303</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>305</v>
@@ -5215,11 +5245,11 @@
       </c>
     </row>
     <row r="67" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A67" s="8" t="s">
+      <c r="A67" s="7" t="s">
         <v>304</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>312</v>
@@ -5253,11 +5283,11 @@
       </c>
     </row>
     <row r="68" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A68" s="8" t="s">
+      <c r="A68" s="7" t="s">
         <v>315</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>317</v>
@@ -5291,11 +5321,11 @@
       </c>
     </row>
     <row r="69" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A69" s="8" t="s">
+      <c r="A69" s="7" t="s">
         <v>316</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>341</v>
@@ -5329,11 +5359,11 @@
       </c>
     </row>
     <row r="70" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A70" s="8" t="s">
+      <c r="A70" s="7" t="s">
         <v>324</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>342</v>
@@ -5367,11 +5397,11 @@
       </c>
     </row>
     <row r="71" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A71" s="8" t="s">
+      <c r="A71" s="7" t="s">
         <v>325</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>345</v>
@@ -5405,11 +5435,11 @@
       </c>
     </row>
     <row r="72" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A72" s="8" t="s">
+      <c r="A72" s="7" t="s">
         <v>326</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>346</v>
@@ -5443,11 +5473,11 @@
       </c>
     </row>
     <row r="73" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A73" s="8" t="s">
+      <c r="A73" s="7" t="s">
         <v>327</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>352</v>
@@ -5481,11 +5511,11 @@
       </c>
     </row>
     <row r="74" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A74" s="8" t="s">
+      <c r="A74" s="7" t="s">
         <v>328</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>353</v>
@@ -5519,11 +5549,11 @@
       </c>
     </row>
     <row r="75" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A75" s="8" t="s">
+      <c r="A75" s="7" t="s">
         <v>329</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>354</v>
@@ -5557,11 +5587,11 @@
       </c>
     </row>
     <row r="76" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A76" s="8" t="s">
+      <c r="A76" s="7" t="s">
         <v>330</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>355</v>
@@ -5595,11 +5625,11 @@
       </c>
     </row>
     <row r="77" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A77" s="8" t="s">
+      <c r="A77" s="7" t="s">
         <v>331</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>356</v>
@@ -5633,11 +5663,11 @@
       </c>
     </row>
     <row r="78" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A78" s="8" t="s">
+      <c r="A78" s="7" t="s">
         <v>332</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>357</v>
@@ -5671,11 +5701,11 @@
       </c>
     </row>
     <row r="79" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A79" s="8" t="s">
+      <c r="A79" s="7" t="s">
         <v>333</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>358</v>
@@ -5709,11 +5739,11 @@
       </c>
     </row>
     <row r="80" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A80" s="8" t="s">
+      <c r="A80" s="7" t="s">
         <v>334</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>359</v>
@@ -5747,11 +5777,11 @@
       </c>
     </row>
     <row r="81" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A81" s="8" t="s">
+      <c r="A81" s="7" t="s">
         <v>335</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>360</v>
@@ -5785,11 +5815,11 @@
       </c>
     </row>
     <row r="82" spans="1:12" x14ac:dyDescent="0.15">
-      <c r="A82" s="8" t="s">
+      <c r="A82" s="7" t="s">
         <v>336</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>361</v>
@@ -5827,7 +5857,7 @@
         <v>396</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>397</v>
@@ -5865,7 +5895,7 @@
         <v>404</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>405</v>
@@ -5903,7 +5933,7 @@
         <v>411</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>422</v>
@@ -5941,7 +5971,7 @@
         <v>412</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>423</v>
@@ -6130,8 +6160,8 @@
       <c r="A91" s="7" t="s">
         <v>450</v>
       </c>
-      <c r="B91" s="1" t="s">
-        <v>11</v>
+      <c r="B91" s="7" t="s">
+        <v>449</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>456</v>
@@ -6166,7 +6196,7 @@
         <v>451</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>457</v>
@@ -6201,7 +6231,7 @@
         <v>452</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>458</v>
@@ -6236,7 +6266,7 @@
         <v>453</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>459</v>
@@ -6271,7 +6301,7 @@
         <v>454</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>460</v>
@@ -6306,7 +6336,7 @@
         <v>455</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>461</v>
@@ -6341,7 +6371,7 @@
         <v>475</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>477</v>
@@ -6376,7 +6406,7 @@
         <v>476</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>478</v>
@@ -6411,7 +6441,7 @@
         <v>483</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>478</v>
@@ -6446,7 +6476,7 @@
         <v>578</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>580</v>
@@ -6481,7 +6511,7 @@
         <v>579</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>581</v>
@@ -6516,7 +6546,7 @@
         <v>591</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>593</v>
@@ -6552,7 +6582,7 @@
         <v>592</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>594</v>
@@ -6587,8 +6617,8 @@
       <c r="A104" s="7" t="s">
         <v>601</v>
       </c>
-      <c r="B104" s="1" t="s">
-        <v>11</v>
+      <c r="B104" s="7" t="s">
+        <v>449</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>602</v>
@@ -6626,7 +6656,7 @@
         <v>610</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>612</v>
@@ -6664,7 +6694,7 @@
         <v>611</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>622</v>
@@ -6702,7 +6732,7 @@
         <v>621</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>623</v>
@@ -6740,7 +6770,7 @@
         <v>632</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>635</v>
@@ -6778,7 +6808,7 @@
         <v>634</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>636</v>
@@ -6816,7 +6846,7 @@
         <v>637</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>638</v>
@@ -6854,7 +6884,7 @@
         <v>651</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>659</v>
@@ -6892,7 +6922,7 @@
         <v>652</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>11</v>
+        <v>449</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>660</v>
@@ -6923,6 +6953,44 @@
       </c>
       <c r="L112" s="7" t="s">
         <v>19</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A113" s="7" t="s">
+        <v>664</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="D113" s="7" t="s">
+        <v>603</v>
+      </c>
+      <c r="E113" s="7" t="s">
+        <v>604</v>
+      </c>
+      <c r="F113" s="1" t="s">
+        <v>667</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>669</v>
+      </c>
+      <c r="I113" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="J113" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K113" s="7" t="s">
+        <v>670</v>
+      </c>
+      <c r="L113" s="1" t="s">
+        <v>36</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
open dml running in parallel
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -2844,7 +2844,7 @@
   <dimension ref="A1:L113"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B105" sqref="B105"/>
+      <selection activeCell="B88" sqref="B88"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -2906,7 +2906,7 @@
         <v>227</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C2" s="1" t="s">
         <v>12</v>
@@ -2944,7 +2944,7 @@
         <v>228</v>
       </c>
       <c r="B3" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C3" s="1" t="s">
         <v>20</v>
@@ -2982,7 +2982,7 @@
         <v>229</v>
       </c>
       <c r="B4" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C4" s="1" t="s">
         <v>25</v>
@@ -3020,7 +3020,7 @@
         <v>230</v>
       </c>
       <c r="B5" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C5" s="7" t="s">
         <v>27</v>
@@ -3058,7 +3058,7 @@
         <v>231</v>
       </c>
       <c r="B6" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C6" s="1" t="s">
         <v>32</v>
@@ -3093,7 +3093,7 @@
         <v>232</v>
       </c>
       <c r="B7" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C7" s="1" t="s">
         <v>33</v>
@@ -3128,7 +3128,7 @@
         <v>233</v>
       </c>
       <c r="B8" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C8" s="1" t="s">
         <v>56</v>
@@ -3163,7 +3163,7 @@
         <v>234</v>
       </c>
       <c r="B9" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C9" s="7" t="s">
         <v>57</v>
@@ -3198,7 +3198,7 @@
         <v>235</v>
       </c>
       <c r="B10" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C10" s="7" t="s">
         <v>58</v>
@@ -3234,7 +3234,7 @@
         <v>236</v>
       </c>
       <c r="B11" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C11" s="7" t="s">
         <v>59</v>
@@ -3270,7 +3270,7 @@
         <v>237</v>
       </c>
       <c r="B12" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C12" s="7" t="s">
         <v>55</v>
@@ -3306,7 +3306,7 @@
         <v>238</v>
       </c>
       <c r="B13" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C13" s="7" t="s">
         <v>60</v>
@@ -3342,7 +3342,7 @@
         <v>239</v>
       </c>
       <c r="B14" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C14" s="7" t="s">
         <v>61</v>
@@ -3378,7 +3378,7 @@
         <v>240</v>
       </c>
       <c r="B15" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C15" s="7" t="s">
         <v>62</v>
@@ -3414,7 +3414,7 @@
         <v>241</v>
       </c>
       <c r="B16" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C16" s="1" t="s">
         <v>74</v>
@@ -3450,7 +3450,7 @@
         <v>242</v>
       </c>
       <c r="B17" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C17" s="7" t="s">
         <v>77</v>
@@ -3486,7 +3486,7 @@
         <v>243</v>
       </c>
       <c r="B18" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C18" s="1" t="s">
         <v>81</v>
@@ -3522,7 +3522,7 @@
         <v>244</v>
       </c>
       <c r="B19" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C19" s="7" t="s">
         <v>82</v>
@@ -3558,7 +3558,7 @@
         <v>245</v>
       </c>
       <c r="B20" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C20" s="7" t="s">
         <v>83</v>
@@ -3594,7 +3594,7 @@
         <v>246</v>
       </c>
       <c r="B21" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C21" s="7" t="s">
         <v>84</v>
@@ -3630,7 +3630,7 @@
         <v>247</v>
       </c>
       <c r="B22" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C22" s="1" t="s">
         <v>92</v>
@@ -3665,7 +3665,7 @@
         <v>248</v>
       </c>
       <c r="B23" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C23" s="7" t="s">
         <v>92</v>
@@ -3700,7 +3700,7 @@
         <v>249</v>
       </c>
       <c r="B24" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C24" s="7" t="s">
         <v>92</v>
@@ -3735,7 +3735,7 @@
         <v>250</v>
       </c>
       <c r="B25" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C25" s="7" t="s">
         <v>92</v>
@@ -3770,7 +3770,7 @@
         <v>251</v>
       </c>
       <c r="B26" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C26" s="7" t="s">
         <v>92</v>
@@ -3805,7 +3805,7 @@
         <v>252</v>
       </c>
       <c r="B27" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C27" s="7" t="s">
         <v>92</v>
@@ -3840,7 +3840,7 @@
         <v>253</v>
       </c>
       <c r="B28" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C28" s="7" t="s">
         <v>110</v>
@@ -3875,7 +3875,7 @@
         <v>254</v>
       </c>
       <c r="B29" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C29" s="7" t="s">
         <v>110</v>
@@ -3911,7 +3911,7 @@
         <v>255</v>
       </c>
       <c r="B30" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C30" s="7" t="s">
         <v>110</v>
@@ -3947,7 +3947,7 @@
         <v>256</v>
       </c>
       <c r="B31" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C31" s="7" t="s">
         <v>110</v>
@@ -3983,7 +3983,7 @@
         <v>257</v>
       </c>
       <c r="B32" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>127</v>
@@ -4021,7 +4021,7 @@
         <v>258</v>
       </c>
       <c r="B33" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C33" s="7" t="s">
         <v>128</v>
@@ -4059,7 +4059,7 @@
         <v>259</v>
       </c>
       <c r="B34" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C34" s="7" t="s">
         <v>129</v>
@@ -4097,7 +4097,7 @@
         <v>260</v>
       </c>
       <c r="B35" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C35" s="7" t="s">
         <v>153</v>
@@ -4135,7 +4135,7 @@
         <v>261</v>
       </c>
       <c r="B36" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C36" s="7" t="s">
         <v>154</v>
@@ -4173,7 +4173,7 @@
         <v>262</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C37" s="7" t="s">
         <v>130</v>
@@ -4211,7 +4211,7 @@
         <v>263</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C38" s="7" t="s">
         <v>131</v>
@@ -4249,7 +4249,7 @@
         <v>264</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C39" s="7" t="s">
         <v>132</v>
@@ -4287,7 +4287,7 @@
         <v>265</v>
       </c>
       <c r="B40" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C40" s="7" t="s">
         <v>133</v>
@@ -4325,7 +4325,7 @@
         <v>266</v>
       </c>
       <c r="B41" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C41" s="7" t="s">
         <v>134</v>
@@ -4363,7 +4363,7 @@
         <v>267</v>
       </c>
       <c r="B42" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C42" s="7" t="s">
         <v>135</v>
@@ -4401,7 +4401,7 @@
         <v>268</v>
       </c>
       <c r="B43" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C43" s="7" t="s">
         <v>160</v>
@@ -4439,7 +4439,7 @@
         <v>269</v>
       </c>
       <c r="B44" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C44" s="7" t="s">
         <v>162</v>
@@ -4477,7 +4477,7 @@
         <v>270</v>
       </c>
       <c r="B45" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C45" s="1" t="s">
         <v>125</v>
@@ -4515,7 +4515,7 @@
         <v>271</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C46" s="7" t="s">
         <v>168</v>
@@ -4553,7 +4553,7 @@
         <v>272</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C47" s="1" t="s">
         <v>177</v>
@@ -4591,7 +4591,7 @@
         <v>273</v>
       </c>
       <c r="B48" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C48" s="7" t="s">
         <v>206</v>
@@ -4629,7 +4629,7 @@
         <v>274</v>
       </c>
       <c r="B49" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C49" s="7" t="s">
         <v>205</v>
@@ -4667,7 +4667,7 @@
         <v>275</v>
       </c>
       <c r="B50" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C50" s="7" t="s">
         <v>209</v>
@@ -4705,7 +4705,7 @@
         <v>276</v>
       </c>
       <c r="B51" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C51" s="7" t="s">
         <v>208</v>
@@ -4743,7 +4743,7 @@
         <v>277</v>
       </c>
       <c r="B52" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C52" s="7" t="s">
         <v>211</v>
@@ -4781,7 +4781,7 @@
         <v>278</v>
       </c>
       <c r="B53" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C53" s="7" t="s">
         <v>210</v>
@@ -4819,7 +4819,7 @@
         <v>279</v>
       </c>
       <c r="B54" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C54" s="7" t="s">
         <v>213</v>
@@ -4857,7 +4857,7 @@
         <v>280</v>
       </c>
       <c r="B55" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C55" s="7" t="s">
         <v>212</v>
@@ -4895,7 +4895,7 @@
         <v>281</v>
       </c>
       <c r="B56" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C56" s="1" t="s">
         <v>181</v>
@@ -4933,7 +4933,7 @@
         <v>282</v>
       </c>
       <c r="B57" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C57" s="1" t="s">
         <v>182</v>
@@ -4971,7 +4971,7 @@
         <v>283</v>
       </c>
       <c r="B58" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C58" s="1" t="s">
         <v>190</v>
@@ -5000,7 +5000,7 @@
         <v>284</v>
       </c>
       <c r="B59" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C59" s="7" t="s">
         <v>190</v>
@@ -5029,7 +5029,7 @@
         <v>285</v>
       </c>
       <c r="B60" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C60" s="7" t="s">
         <v>192</v>
@@ -5056,7 +5056,7 @@
         <v>286</v>
       </c>
       <c r="B61" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>191</v>
@@ -5085,7 +5085,7 @@
         <v>287</v>
       </c>
       <c r="B62" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C62" s="7" t="s">
         <v>191</v>
@@ -5114,7 +5114,7 @@
         <v>288</v>
       </c>
       <c r="B63" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C63" s="1" t="s">
         <v>193</v>
@@ -5141,7 +5141,7 @@
         <v>291</v>
       </c>
       <c r="B64" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>292</v>
@@ -5176,7 +5176,7 @@
         <v>298</v>
       </c>
       <c r="B65" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>299</v>
@@ -5211,7 +5211,7 @@
         <v>303</v>
       </c>
       <c r="B66" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>305</v>
@@ -5249,7 +5249,7 @@
         <v>304</v>
       </c>
       <c r="B67" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>312</v>
@@ -5287,7 +5287,7 @@
         <v>315</v>
       </c>
       <c r="B68" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C68" s="7" t="s">
         <v>317</v>
@@ -5325,7 +5325,7 @@
         <v>316</v>
       </c>
       <c r="B69" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C69" s="7" t="s">
         <v>341</v>
@@ -5363,7 +5363,7 @@
         <v>324</v>
       </c>
       <c r="B70" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C70" s="7" t="s">
         <v>342</v>
@@ -5401,7 +5401,7 @@
         <v>325</v>
       </c>
       <c r="B71" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C71" s="7" t="s">
         <v>345</v>
@@ -5439,7 +5439,7 @@
         <v>326</v>
       </c>
       <c r="B72" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C72" s="7" t="s">
         <v>346</v>
@@ -5477,7 +5477,7 @@
         <v>327</v>
       </c>
       <c r="B73" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C73" s="7" t="s">
         <v>352</v>
@@ -5515,7 +5515,7 @@
         <v>328</v>
       </c>
       <c r="B74" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C74" s="7" t="s">
         <v>353</v>
@@ -5553,7 +5553,7 @@
         <v>329</v>
       </c>
       <c r="B75" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C75" s="7" t="s">
         <v>354</v>
@@ -5591,7 +5591,7 @@
         <v>330</v>
       </c>
       <c r="B76" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C76" s="7" t="s">
         <v>355</v>
@@ -5629,7 +5629,7 @@
         <v>331</v>
       </c>
       <c r="B77" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C77" s="7" t="s">
         <v>356</v>
@@ -5667,7 +5667,7 @@
         <v>332</v>
       </c>
       <c r="B78" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C78" s="7" t="s">
         <v>357</v>
@@ -5705,7 +5705,7 @@
         <v>333</v>
       </c>
       <c r="B79" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C79" s="7" t="s">
         <v>358</v>
@@ -5743,7 +5743,7 @@
         <v>334</v>
       </c>
       <c r="B80" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C80" s="7" t="s">
         <v>359</v>
@@ -5781,7 +5781,7 @@
         <v>335</v>
       </c>
       <c r="B81" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C81" s="7" t="s">
         <v>360</v>
@@ -5819,7 +5819,7 @@
         <v>336</v>
       </c>
       <c r="B82" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C82" s="7" t="s">
         <v>361</v>
@@ -5857,7 +5857,7 @@
         <v>396</v>
       </c>
       <c r="B83" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>397</v>
@@ -5895,7 +5895,7 @@
         <v>404</v>
       </c>
       <c r="B84" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C84" s="1" t="s">
         <v>405</v>
@@ -5933,7 +5933,7 @@
         <v>411</v>
       </c>
       <c r="B85" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C85" s="1" t="s">
         <v>422</v>
@@ -5971,7 +5971,7 @@
         <v>412</v>
       </c>
       <c r="B86" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C86" s="7" t="s">
         <v>423</v>
@@ -6161,7 +6161,7 @@
         <v>450</v>
       </c>
       <c r="B91" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C91" s="1" t="s">
         <v>456</v>
@@ -6196,7 +6196,7 @@
         <v>451</v>
       </c>
       <c r="B92" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C92" s="1" t="s">
         <v>457</v>
@@ -6231,7 +6231,7 @@
         <v>452</v>
       </c>
       <c r="B93" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C93" s="1" t="s">
         <v>458</v>
@@ -6266,7 +6266,7 @@
         <v>453</v>
       </c>
       <c r="B94" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C94" s="1" t="s">
         <v>459</v>
@@ -6301,7 +6301,7 @@
         <v>454</v>
       </c>
       <c r="B95" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C95" s="1" t="s">
         <v>460</v>
@@ -6336,7 +6336,7 @@
         <v>455</v>
       </c>
       <c r="B96" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C96" s="1" t="s">
         <v>461</v>
@@ -6371,7 +6371,7 @@
         <v>475</v>
       </c>
       <c r="B97" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C97" s="1" t="s">
         <v>477</v>
@@ -6406,7 +6406,7 @@
         <v>476</v>
       </c>
       <c r="B98" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C98" s="1" t="s">
         <v>478</v>
@@ -6441,7 +6441,7 @@
         <v>483</v>
       </c>
       <c r="B99" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C99" s="7" t="s">
         <v>478</v>
@@ -6476,7 +6476,7 @@
         <v>578</v>
       </c>
       <c r="B100" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C100" s="1" t="s">
         <v>580</v>
@@ -6511,7 +6511,7 @@
         <v>579</v>
       </c>
       <c r="B101" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C101" s="7" t="s">
         <v>581</v>
@@ -6546,7 +6546,7 @@
         <v>591</v>
       </c>
       <c r="B102" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C102" s="7" t="s">
         <v>593</v>
@@ -6582,7 +6582,7 @@
         <v>592</v>
       </c>
       <c r="B103" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C103" s="7" t="s">
         <v>594</v>
@@ -6618,7 +6618,7 @@
         <v>601</v>
       </c>
       <c r="B104" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C104" s="1" t="s">
         <v>602</v>
@@ -6656,7 +6656,7 @@
         <v>610</v>
       </c>
       <c r="B105" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C105" s="1" t="s">
         <v>612</v>
@@ -6694,7 +6694,7 @@
         <v>611</v>
       </c>
       <c r="B106" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C106" s="1" t="s">
         <v>622</v>
@@ -6732,7 +6732,7 @@
         <v>621</v>
       </c>
       <c r="B107" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C107" s="7" t="s">
         <v>623</v>
@@ -6770,7 +6770,7 @@
         <v>632</v>
       </c>
       <c r="B108" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C108" s="1" t="s">
         <v>635</v>
@@ -6808,7 +6808,7 @@
         <v>634</v>
       </c>
       <c r="B109" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C109" s="7" t="s">
         <v>636</v>
@@ -6846,7 +6846,7 @@
         <v>637</v>
       </c>
       <c r="B110" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C110" s="7" t="s">
         <v>638</v>
@@ -6884,7 +6884,7 @@
         <v>651</v>
       </c>
       <c r="B111" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C111" s="1" t="s">
         <v>659</v>
@@ -6922,7 +6922,7 @@
         <v>652</v>
       </c>
       <c r="B112" s="7" t="s">
-        <v>449</v>
+        <v>11</v>
       </c>
       <c r="C112" s="7" t="s">
         <v>660</v>

</xml_diff>

<commit_message>
update some case data
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -2411,10 +2411,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>select * from $scalar055 where amount=888.88</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_110.csv</t>
   </si>
   <si>
@@ -2464,6 +2460,10 @@
   </si>
   <si>
     <t>select id,age,gender,hobby,color_index$distance from vector($mixindex018, color, array[0.009107396006584167,-0.4928479492664337,-0.06084398180246353,0.11279209703207016,0.42720580101013184,-0.5535244345664978,-0.051339954137802124,0.3442928194999695,0.397807240486145,0.14437393844127655,-0.27258825302124023,0.11299128085374832,0.26662662625312805,-0.3028406798839569,-0.06034494936466217,-0.20874223113059998,0.710351824760437,0.03114473819732666,-0.10010837763547897,-0.499957799911499,-0.3172328472137451,0.18967600166797638,0.16708506643772125,-0.31831443309783936,-0.3038794696331024,0.517365038394928,-0.1310274302959442,0.6051051020622253,-0.29701799154281616,-0.11700791120529175,-0.49527180194854736,0.3499431014060974,-0.05310584604740143,0.11840163171291351,-0.6476613283157349,-0.40672868490219116,0.15504536032676697,-0.04425550997257233,-0.017758861184120178,-0.4650961756706238,-0.367722749710083,0.4912892282009125,0.15679343044757843,-1.2024909257888794,-0.6475555896759033,0.8445031642913818,-0.3021777868270874,0.0012783706188201904,-0.1028386726975441,-0.028430849313735962,0.4390820562839508,0.17291557788848877,0.02308507263660431,-0.2666246294975281,0.030758768320083618,0.3070322275161743,0.7922346591949463,0.15251073241233826,0.3876311779022217,-0.12918725609779358,0.5775445699691772,0.13809040188789368,0.3011755347251892,-0.08841019868850708,-0.2804226875305176,0.08000586181879044,0.23992058634757996,0.30137330293655396,-0.573534369468689,-0.08557131141424179,-0.009991265833377838,0.22057701647281647,-0.07465316355228424,-0.1380939483642578,0.12757709622383118,-0.1524963080883026,-0.21346122026443481,-0.21207493543624878,-0.299119770526886,-0.105656199157238,0.2978556156158447,0.27103662490844727,-0.04677818715572357,-0.25942736864089966,0.23926180601119995,0.06485702842473984,-0.2326173037290573,-0.7795956134796143,0.5515224933624268,-0.13598020374774933,-0.3016166687011719,-0.23002196848392487,-5.020496845245361,1.1768553256988525,0.04210896044969559,0.05429087206721306,-0.12462489306926727,-0.2512921392917633,0.025492563843727112,-0.014712274074554443,0.3395729660987854,0.36077940464019775,0.710265040397644,0.5866747498512268,0.3867844343185425,0.16563571989536285,-2.2621219158172607,-0.31919386982917786,-0.29929596185684204,-0.1239459365606308,-0.019464053213596344,-0.18152916431427002,0.015370100736618042,-0.39437994360923767,-0.3952904939651489,-0.17863686382770538,0.3756665587425232,0.01915770024061203,-0.0487205907702446,0.5403110980987549,0.13948170840740204,0.7490887641906738,0.218780517578125,0.21333663165569305,0.6106190085411072,-0.5787690877914429,0.005233213305473328,-0.02014821767807007,-0.37207454442977905,0.04737117886543274,0.3805462121963501,0.022129982709884644,-0.08685516566038132,0.8918148279190063,0.332944393157959,-0.17890742421150208,-0.01971307396888733,-0.49113523960113525,-0.16974413394927979,0.29028767347335815,-0.0854928120970726,-0.28040117025375366,0.27752572298049927,0.19523702561855316,-0.010701179504394531,0.41232433915138245,-0.2981152832508087,0.17831067740917206,0.23491880297660828,0.5166872143745422,0.03726338595151901,-0.09167103469371796,-0.14614176750183105,0.0835254117846489,-0.526052713394165,0.5634927749633789,0.4244139492511749,0.08627873659133911,0.11286911368370056,-0.09144455194473267,0.19640317559242249,-0.28446879982948303,-0.14722681045532227,-0.15440787374973297,0.38722527027130127,0.2799495756626129,0.2579476833343506,0.07801324129104614,-0.03614184260368347,0.2691837549209595,-0.22063779830932617,0.20414650440216064,0.290392130613327,-0.23576216399669647,0.6217473745346069,-0.36090806126594543,-0.5171005129814148,-0.0978025570511818,-0.22199128568172455,0.11597487330436707,-0.10627104341983795,0.0140666663646698,-0.3552021086215973,0.04552648216485977,0.028643697500228882,-0.2697099447250366,-0.08528557419776917,-0.3565848469734192,-0.6836068034172058,0.4241693317890167,0.3769601583480835,-0.3473547399044037,-0.28350770473480225,0.4194734990596771,0.16857166588306427,0.24369701743125916,0.7187827229499817,-0.24069659411907196,-0.612932026386261,-0.02567557990550995,0.025800958275794983,-0.2763204872608185,0.06153678894042969,0.42983344197273254,-0.27653318643569946,0.07124429941177368,-0.21047277748584747,-0.19868281483650208,-0.40652528405189514,-0.2593531012535095,0.35989561676979065,0.7571883797645569,0.6407842636108398,0.29625385999679565,0.4905804395675659,-0.11757611483335495,-0.15926161408424377,0.05945210158824921,0.9470091462135315,-0.2651394009590149,0.24507103860378265,0.012639820575714111,-0.16477082669734955,0.023227810859680176,0.3517795503139496,0.061285004019737244,0.23400992155075073,-0.004913773387670517,0.10474497079849243,0.28454095125198364,0.2646726965904236,0.056223608553409576,0.14024418592453003,0.09913889318704605,0.37895309925079346,0.4080517888069153,0.23690679669380188,-0.9799992442131042,0.6079041361808777,-0.8063328862190247,-0.18007591366767883,0.4238743185997009,0.5677311420440674,0.07879464328289032,-0.6451236009597778,0.3615572452545166,-0.6502392292022705,-0.13250525295734406,0.022514693439006805,0.23416417837142944,-0.31921306252479553,0.015400782227516174,0.3049747347831726,-0.49025920033454895,0.6232213377952576,-0.17872992157936096,0.22888170182704926,0.06563788652420044,-0.09811440110206604,0.5739450454711914,0.19145318865776062,0.19296371936798096,0.1447419375181198,0.6271354556083679,-0.40667158365249634,0.14535176753997803,0.08282049000263214,-0.2226463258266449,0.19218046963214874,0.18990464508533478,0.366453617811203,0.1181904524564743,0.31326085329055786,0.2777858078479767,0.18976512551307678,0.12058664858341217,0.3834364712238312,-0.25943732261657715,0.15866270661354065,-0.14582546055316925,0.2993849217891693,0.3625524640083313,-0.5657874345779419,0.3584221601486206,0.6659886837005615,0.5365152359008789,0.15160009264945984,-0.0038372427225112915,-0.03198322653770447,-0.41171130537986755,0.35392409563064575,0.4899391531944275,-0.44131115078926086,-0.03127241134643555,-0.08564724773168564,-0.2810729742050171,-0.1650094985961914,0.41276872158050537,-0.20266728103160858,-0.21721073985099792,0.06289903819561005,-0.1000848263502121,0.3060847520828247,-0.1798524409532547,-0.053416907787323,-0.17533081769943237,0.4803808927536011,0.6472082734107971,-0.20990946888923645,-0.08272083848714828,0.2603752315044403,0.2435430884361267,0.8928165435791016,0.04669277369976044,0.06500576436519623,0.0932016521692276,0.4320862591266632,-0.19006873667240143,-0.4583078622817993,-0.06959453225135803,0.41687387228012085,1.279518961906433,-0.09231052547693253,0.39603978395462036,0.4426204264163971,0.1414766013622284,0.14081603288650513,0.029098331928253174,-0.0008250568062067032,-0.04960125684738159,0.10457373410463333,0.5750452876091003,-0.23702768981456757,0.07400791347026825,-0.39593395590782166,0.2875250577926636,0.40632858872413635,0.4273437261581421,-0.15563148260116577,-0.1943039447069168,0.09682011604309082,0.2771073579788208,-0.17696169018745422,-0.15394936501979828,-0.028617314994335175,-0.6125500202178955,0.055850833654403687,-0.33313047885894775,-0.18644365668296814,0.05475170910358429,0.08947843313217163,-0.07653182744979858,0.09828981757164001,-0.03744521737098694,-0.09890225529670715,0.3104325830936432,0.3743216395378113,0.7847214937210083,0.22328320145606995,-0.007173389196395874,0.2743714451789856,0.3419463038444519,-0.4041624963283539,0.8219678401947021,-0.937566339969635,-0.0877365693449974,0.08319441229104996,0.519494891166687,0.14611385762691498,0.6832436919212341,0.08052428811788559,0.4532940685749054,-0.11158505082130432,0.05747853219509125,-0.03627094626426697,0.29975807666778564,0.3184080719947815,-0.15185518562793732,-0.17107611894607544,-0.26622259616851807,-0.041283462196588516,0.2775959074497223,0.5768389701843262,-0.19857929646968842,-0.383053183555603,-0.4868699014186859,0.3679580092430115,0.31410154700279236,0.45399945974349976,0.565982460975647,-0.9887039661407471,-0.5410878658294678,-0.25793322920799255,-0.4151421785354614,0.9581260085105896,0.08737964928150177,0.12770259380340576,0.17853334546089172,-0.47929897904396057,-0.18773919343948364,-0.06778784096240997,0.2790369987487793,0.3038453459739685,-0.00035012513399124146,0.21557708084583282,-0.2987268567085266,-0.37862226366996765,0.11563920229673386,0.37216106057167053,0.07540548592805862,-0.14644283056259155,0.36704716086387634,0.27644112706184387,0.23733626306056976,-0.15499460697174072,0.18270283937454224,0.286896288394928,0.0611887089908123,-0.003465220332145691,-0.44345101714134216,-0.48094767332077026,-0.05870349705219269,0.2203047126531601,0.23658716678619385,0.14524224400520325,-0.3096632957458496,-0.42239847779273987,0.14180953800678253,-1.9080333709716797,0.7268998026847839,0.21734172105789185,0.3595874309539795,-0.24850676953792572,-0.0687989890575409,-0.2876971960067749,-0.008909806609153748,0.06251184642314911,0.17282895743846893,-0.24134333431720734,-0.34526604413986206,-0.6466650366783142,0.42585867643356323,0.5730605125427246,0.02659779042005539,0.3097115755081177,0.29858189821243286,-0.07963889837265015,-0.2749827802181244,-0.03155626356601715,-0.037864506244659424,0.11886607110500336,0.0742151141166687,0.454728901386261,0.11392711102962494,-0.0018827617168426514,-0.6696452498435974,0.3057352304458618,0.18775613605976105,0.07171911001205444,0.1750405877828598,-0.2657383978366852,0.24411165714263916,0.2512362003326416,-0.10027620196342468,0.3601529002189636,0.37912803888320923,-0.06990914046764374,-0.3299768567085266,-0.125762477517128,-0.2828892767429352,0.15549014508724213,0.13161194324493408,0.39875492453575134,-0.4680383801460266,-0.13426533341407776,0.2584708333015442,0.01619536429643631,0.26572245359420776,-0.3058027923107147,0.0349903404712677,-0.5298135280609131,-0.5118231177330017,0.35788029432296753,0.25099503993988037,-0.3409276306629181,0.0350998193025589,0.12917760014533997,0.04360932856798172,0.03863629698753357,-0.12423983961343765,-0.44539687037467957,0.06586220115423203,0.29936468601226807,-0.7707462310791016,-0.130367249250412,0.18743553757667542,-0.2837158441543579,0.07794137299060822,-0.24770815670490265,0.4286563992500305,-0.13582590222358704,0.13121500611305237,-0.001750364899635315,0.3049774765968323,-0.39047953486442566,0.24318626523017883,-0.4263252913951874,0.2714003324508667,0.17210617661476135,0.6087738871574402,-0.18345880508422852,0.11825743317604065], 10) where age&gt;1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select id,name,age,gmt,price,amount,address,birthday,create_time,update_time,zip_code,is_delete from $scalar055 where amount=888.88</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -2843,8 +2843,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:L113"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A71" workbookViewId="0">
-      <selection activeCell="B88" sqref="B88"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B20" sqref="B20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -6887,7 +6887,7 @@
         <v>11</v>
       </c>
       <c r="C111" s="1" t="s">
-        <v>659</v>
+        <v>658</v>
       </c>
       <c r="D111" s="7" t="s">
         <v>603</v>
@@ -6908,10 +6908,10 @@
         <v>656</v>
       </c>
       <c r="J111" s="1" t="s">
+        <v>671</v>
+      </c>
+      <c r="K111" s="7" t="s">
         <v>657</v>
-      </c>
-      <c r="K111" s="7" t="s">
-        <v>658</v>
       </c>
       <c r="L111" s="7" t="s">
         <v>19</v>
@@ -6925,7 +6925,7 @@
         <v>11</v>
       </c>
       <c r="C112" s="7" t="s">
-        <v>660</v>
+        <v>659</v>
       </c>
       <c r="D112" s="7" t="s">
         <v>603</v>
@@ -6940,16 +6940,16 @@
         <v>654</v>
       </c>
       <c r="H112" s="7" t="s">
-        <v>661</v>
+        <v>660</v>
       </c>
       <c r="I112" s="1" t="s">
         <v>656</v>
       </c>
       <c r="J112" s="7" t="s">
+        <v>661</v>
+      </c>
+      <c r="K112" s="7" t="s">
         <v>662</v>
-      </c>
-      <c r="K112" s="7" t="s">
-        <v>663</v>
       </c>
       <c r="L112" s="7" t="s">
         <v>19</v>
@@ -6957,13 +6957,13 @@
     </row>
     <row r="113" spans="1:12" x14ac:dyDescent="0.15">
       <c r="A113" s="7" t="s">
+        <v>663</v>
+      </c>
+      <c r="B113" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C113" s="1" t="s">
         <v>664</v>
-      </c>
-      <c r="B113" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C113" s="1" t="s">
-        <v>665</v>
       </c>
       <c r="D113" s="7" t="s">
         <v>603</v>
@@ -6972,22 +6972,22 @@
         <v>604</v>
       </c>
       <c r="F113" s="1" t="s">
+        <v>666</v>
+      </c>
+      <c r="G113" s="1" t="s">
+        <v>665</v>
+      </c>
+      <c r="H113" s="1" t="s">
+        <v>668</v>
+      </c>
+      <c r="I113" s="1" t="s">
         <v>667</v>
       </c>
-      <c r="G113" s="1" t="s">
-        <v>666</v>
-      </c>
-      <c r="H113" s="1" t="s">
+      <c r="J113" s="1" t="s">
+        <v>670</v>
+      </c>
+      <c r="K113" s="7" t="s">
         <v>669</v>
-      </c>
-      <c r="I113" s="1" t="s">
-        <v>668</v>
-      </c>
-      <c r="J113" s="1" t="s">
-        <v>671</v>
-      </c>
-      <c r="K113" s="7" t="s">
-        <v>670</v>
       </c>
       <c r="L113" s="1" t="s">
         <v>36</v>

</xml_diff>

<commit_message>
add case about update and delete with index or key logic filter
</commit_message>
<xml_diff>
--- a/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
+++ b/src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/sql_updatedelete_cases.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1399" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1487" uniqueCount="767">
   <si>
     <t>Expected_result</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -2652,6 +2652,166 @@
   </si>
   <si>
     <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_121.csv</t>
+  </si>
+  <si>
+    <t>updel_122</t>
+  </si>
+  <si>
+    <t>updel_123</t>
+  </si>
+  <si>
+    <t>主键等值逻辑与删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键等值逻辑或删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_124</t>
+  </si>
+  <si>
+    <t>updel_125</t>
+  </si>
+  <si>
+    <t>索引列等值逻辑与删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>索引列等值逻辑或删除</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $scalar058 where id=8 and id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>0</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar058 where id=8 and id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_122.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_123.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_124.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_125.csv</t>
+  </si>
+  <si>
+    <t>delete from $scalar058 where id=8 or id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $scalar058 where age=-18 and age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>delete from $scalar058 where age=-18 or age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar058 where id=8 or id=28 or id=18 or id=38</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar058 where age=-18 and age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $scalar058 where age=-18 and age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $scalar058 where age=-18 or age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>updel_126</t>
+  </si>
+  <si>
+    <t>updel_127</t>
+  </si>
+  <si>
+    <t>updel_128</t>
+  </si>
+  <si>
+    <t>updel_129</t>
+  </si>
+  <si>
+    <t>主键等值逻辑与更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>主键等值逻辑或更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>索引列等值逻辑与更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>索引列等值逻辑或更新</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $scalar058 set age=888 where id=8 and id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $scalar058 where id=8 and id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_126.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_127.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_128.csv</t>
+  </si>
+  <si>
+    <t>src/test/resources/io.dingodb.test/testdata/cases/dml/updatedelete/expectedresult/updatedelete_129.csv</t>
+  </si>
+  <si>
+    <t>update $scalar058 set age=888 where id=8 or id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select age from $scalar058 where id=8 or id=28</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $scalar058 set age=888 where age=-18 and age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>update $scalar058 set age=888 where age=-18 or age=18</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>4</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>select * from $scalar058 where age=-18 or age=18 or age=888</t>
+    <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -3028,10 +3188,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L122"/>
+  <dimension ref="A1:L130"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
-      <selection activeCell="I128" sqref="I128"/>
+    <sheetView tabSelected="1" topLeftCell="D94" workbookViewId="0">
+      <selection activeCell="H109" sqref="H109"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -3043,7 +3203,7 @@
     <col min="5" max="5" width="11.875" style="1" customWidth="1"/>
     <col min="6" max="6" width="14.75" style="1" customWidth="1"/>
     <col min="7" max="7" width="22.125" style="1" customWidth="1"/>
-    <col min="8" max="8" width="60.625" style="1" customWidth="1"/>
+    <col min="8" max="8" width="88.375" style="1" customWidth="1"/>
     <col min="9" max="9" width="17" style="1" bestFit="1" customWidth="1"/>
     <col min="10" max="10" width="38" style="1" customWidth="1"/>
     <col min="11" max="12" width="19.5" style="1" bestFit="1" customWidth="1"/>
@@ -7510,6 +7670,287 @@
         <v>722</v>
       </c>
       <c r="L122" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A123" s="7" t="s">
+        <v>723</v>
+      </c>
+      <c r="B123" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C123" s="1" t="s">
+        <v>725</v>
+      </c>
+      <c r="D123" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F123" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G123" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H123" s="1" t="s">
+        <v>731</v>
+      </c>
+      <c r="I123" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="J123" s="1" t="s">
+        <v>733</v>
+      </c>
+      <c r="K123" s="7" t="s">
+        <v>734</v>
+      </c>
+      <c r="L123" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="124" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A124" s="7" t="s">
+        <v>724</v>
+      </c>
+      <c r="B124" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C124" s="7" t="s">
+        <v>726</v>
+      </c>
+      <c r="D124" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E124" s="7"/>
+      <c r="F124" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G124" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H124" s="7" t="s">
+        <v>738</v>
+      </c>
+      <c r="I124" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="J124" s="7" t="s">
+        <v>742</v>
+      </c>
+      <c r="K124" s="7" t="s">
+        <v>735</v>
+      </c>
+      <c r="L124" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="125" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A125" s="7" t="s">
+        <v>727</v>
+      </c>
+      <c r="B125" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C125" s="1" t="s">
+        <v>729</v>
+      </c>
+      <c r="D125" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F125" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G125" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H125" s="7" t="s">
+        <v>739</v>
+      </c>
+      <c r="I125" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="J125" s="1" t="s">
+        <v>744</v>
+      </c>
+      <c r="K125" s="7" t="s">
+        <v>736</v>
+      </c>
+      <c r="L125" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="126" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A126" s="7" t="s">
+        <v>728</v>
+      </c>
+      <c r="B126" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C126" s="7" t="s">
+        <v>730</v>
+      </c>
+      <c r="D126" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F126" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G126" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H126" s="7" t="s">
+        <v>740</v>
+      </c>
+      <c r="I126" s="1" t="s">
+        <v>745</v>
+      </c>
+      <c r="J126" s="1" t="s">
+        <v>746</v>
+      </c>
+      <c r="K126" s="7" t="s">
+        <v>737</v>
+      </c>
+      <c r="L126" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="127" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A127" s="7" t="s">
+        <v>747</v>
+      </c>
+      <c r="B127" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C127" s="7" t="s">
+        <v>751</v>
+      </c>
+      <c r="D127" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F127" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G127" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H127" s="7" t="s">
+        <v>755</v>
+      </c>
+      <c r="I127" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="J127" s="1" t="s">
+        <v>756</v>
+      </c>
+      <c r="K127" s="7" t="s">
+        <v>757</v>
+      </c>
+      <c r="L127" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="128" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A128" s="7" t="s">
+        <v>748</v>
+      </c>
+      <c r="B128" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C128" s="7" t="s">
+        <v>752</v>
+      </c>
+      <c r="D128" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F128" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G128" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H128" s="7" t="s">
+        <v>761</v>
+      </c>
+      <c r="I128" s="1" t="s">
+        <v>741</v>
+      </c>
+      <c r="J128" s="7" t="s">
+        <v>762</v>
+      </c>
+      <c r="K128" s="7" t="s">
+        <v>758</v>
+      </c>
+      <c r="L128" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="129" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A129" s="7" t="s">
+        <v>749</v>
+      </c>
+      <c r="B129" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C129" s="7" t="s">
+        <v>753</v>
+      </c>
+      <c r="D129" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F129" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G129" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H129" s="7" t="s">
+        <v>763</v>
+      </c>
+      <c r="I129" s="1" t="s">
+        <v>732</v>
+      </c>
+      <c r="J129" s="1" t="s">
+        <v>743</v>
+      </c>
+      <c r="K129" s="7" t="s">
+        <v>759</v>
+      </c>
+      <c r="L129" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="130" spans="1:12" x14ac:dyDescent="0.15">
+      <c r="A130" s="7" t="s">
+        <v>750</v>
+      </c>
+      <c r="B130" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="C130" s="7" t="s">
+        <v>754</v>
+      </c>
+      <c r="D130" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="F130" s="7" t="s">
+        <v>713</v>
+      </c>
+      <c r="G130" s="7" t="s">
+        <v>616</v>
+      </c>
+      <c r="H130" s="7" t="s">
+        <v>764</v>
+      </c>
+      <c r="I130" s="7" t="s">
+        <v>765</v>
+      </c>
+      <c r="J130" s="7" t="s">
+        <v>766</v>
+      </c>
+      <c r="K130" s="7" t="s">
+        <v>760</v>
+      </c>
+      <c r="L130" s="7" t="s">
         <v>19</v>
       </c>
     </row>

</xml_diff>